<commit_message>
Updates rbdd data package to remove duplicated recaps and releases
</commit_message>
<xml_diff>
--- a/data-raw/RBDD_RST_DRAFT_Metadata_form_022823.xlsx
+++ b/data-raw/RBDD_RST_DRAFT_Metadata_form_022823.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/CVPIA/data-stewardship/EDI_data_repos_to_upload/rbdd-rst-edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323F01DF-18CB-B948-93F8-43DA5FFB9622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B6B199-7013-8440-A031-21C27B80FC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="1600" windowWidth="25520" windowHeight="15280" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="1600" windowWidth="25520" windowHeight="15280" tabRatio="834" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="306">
   <si>
     <t>first_name</t>
   </si>
@@ -950,6 +950,9 @@
   <si>
     <t>Interagency Agreement R20PG00061 Between
 U.S Department of the Interior, Bureau of Reclamation And U.S. Fish and Wildlife Service For Fish Monitoring Activities in Sacramento River, Clear Creek, and Battle Creek</t>
+  </si>
+  <si>
+    <t>chinook</t>
   </si>
 </sst>
 </file>
@@ -3570,10 +3573,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3612,26 +3615,31 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3777,7 +3785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>